<commit_message>
creation of qa pairs for extractive qa task
</commit_message>
<xml_diff>
--- a/extractions-from-paper/synthetic_procedures.xlsx
+++ b/extractions-from-paper/synthetic_procedures.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="96">
   <si>
     <t>Label</t>
   </si>
@@ -40,19 +40,16 @@
     <t>To a 20mL vial with a Teflon stir bar, diol (1.05 equiv) and dicarboxylic acid (1 equiv) were added. The vial was then fitted with a septum cap and purged with nitrogen. The vial is heated to 150 °C for 1 hour under 1 atm of nitrogen, followed by heating to 175 °C for 1 hour before being placed under vacuum (~10 torr) and cooled to 150 °C for an additional 2 hours. Following that, the vial was refilled with nitrogen (1 atm) and titanium (IV) isopropoxide (0.02 equiv) was added. The reaction was allowed to stir for 30 min before being placed back under vacuum for 12 hours and increasing the temperature to 180 °C.</t>
   </si>
   <si>
-    <t>step-growth polycondansation (esterification)</t>
-  </si>
-  <si>
-    <t>Homopolymer</t>
-  </si>
-  <si>
-    <t>Melt</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Polyester</t>
+    <t>polycondensation</t>
+  </si>
+  <si>
+    <t>homopolymer</t>
+  </si>
+  <si>
+    <t>melt</t>
+  </si>
+  <si>
+    <t>polyester</t>
   </si>
   <si>
     <t>M2</t>
@@ -61,9 +58,6 @@
     <t>To a 20mL vial with a Teflon stir bar, diol (1.01 to 1.1 equiv) and dicarboxylic acid (1 equiv) were added. The vial was then fitted with a septum cap and purged with nitrogen. The vial was heated to 180 °C for 1.5 hours under 1 atm of nitrogen. Titanium (IV) isopropoxide (0.02 equiv) was added, and the reaction was allowed to stir for 30 minutes. Vacuum (~25 torr) was introduced, and the reaction was heated to 200 °C for 1 hour. The reaction temperature was increased to 250 °C, and reacted overnight. The vial was refilled with nitrogen (1 atm), cooled to 200 °C, and additional titanium isopropoxide (0.02 equiv) was added and allowed to stir for 1 hour. Vacuum was reintroduced, and the temperature was increased to 350C for an additional 16 hours.</t>
   </si>
   <si>
-    <t>Polycondansation</t>
-  </si>
-  <si>
     <t>Ti(OiPr)₄</t>
   </si>
   <si>
@@ -217,9 +211,6 @@
     <t>To a 20mL vial with a Teflon stir bar, diol (1 equiv), dimethyl carbonate (2 equiv), and DMAP (0.01 equiv) were added. The vial was then fitted with a septum cap and purged with nitrogen. The vial was heated to 75 °C for 3 hours, followed by 95 °C for 2 hours under 1 atm of nitrogen. The vial was then placed under vacuum (~10 torr) and heated to 1o5 °C overnight.</t>
   </si>
   <si>
-    <t>polycondensation</t>
-  </si>
-  <si>
     <t>DMAP</t>
   </si>
   <si>
@@ -250,10 +241,10 @@
     <t>A vial with a septum cap and Teflon stir bar was prepared for the reaction by drying it in an oven overnight, then purged with nitrogen and then chilled (0 °C). Diol (1 equiv), diacid chloride (1 equiv), TCE (1 M) then were added to the vial. The reaction was initiated with a the slow addition (over 10 min) of pyridine(8 equiv) resulting in solid formation. After 10 min, the water bath was removed, and stirred overnight. The resulting mixture was poured into methanol. The precipitated polymer was collected with vacuum filtration and dried in vacuo to give a solid.</t>
   </si>
   <si>
-    <t>Acid-chloride polycondensation</t>
-  </si>
-  <si>
-    <t>Solution</t>
+    <t>acid-chloride polycondensation</t>
+  </si>
+  <si>
+    <t>solution</t>
   </si>
   <si>
     <t>M32</t>
@@ -262,7 +253,7 @@
     <t>In a 20mL vial, diol (1 equiv) was dissolved in solvent (water or DMF, 7.5mL) with base (1.3 equiv) and a SpinPlus stir bar was added. In a second 20mL vial, acid chloride (1.1mL) was added to a second solvent immiscible with the first (Diethyl Ether, Diisopropyl Ether, Hexanes, or Cyclohexane, 7.5mL). After dissolution of the acid chloride, the solution was added dropwise to the stirring (600 rpm) diol solution. The resulting interfacial reaction was left stirring overnight, and the resulting polymer was precipitated into methanol (200mL).</t>
   </si>
   <si>
-    <t>Interface</t>
+    <t>solution interface</t>
   </si>
   <si>
     <t>M33</t>
@@ -271,16 +262,16 @@
     <t>In a nitrogen atmosphere glovebox, the following steps were performed. To a 20mL vial with a Teflon stir bar, THF (6.5 mL), monomer (1000 equiv) and TBD catalyst (5 equiv) were added and mixed. Subsequently, benzyl alcohol (initiator, 20 equiv) was added, and the reaction was capped and stirred for 20 hours. The reaction was uncapped, and benzoic acid (40 equiv) was added as a quenching agent and subsequently removed from the glovebox.</t>
   </si>
   <si>
-    <t>Ring-opening polymerisation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copolymer/Homopolymer </t>
+    <t>ring-opening polymerisation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">copolymer/homopolymer </t>
   </si>
   <si>
     <t>TBD</t>
   </si>
   <si>
-    <t>Varied</t>
+    <t>polymer</t>
   </si>
   <si>
     <t>M34</t>
@@ -304,7 +295,7 @@
     <t>To a 20mL vial with a Teflon Stir bar, monomers (1000 equiv, 500 equiv), triphephenyl bismuth (30 equiv), and tin octoate (10 equiv) were added. The reaction was stirred at 110 °C for 20 hours.</t>
   </si>
   <si>
-    <t>Copolymer</t>
+    <t>copolymer</t>
   </si>
   <si>
     <t>Sn(Oct)₂, Ph₃Bi</t>
@@ -339,12 +330,18 @@
       <name val="Times Roman"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -357,16 +354,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -383,10 +380,10 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -406,6 +403,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -557,9 +555,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -639,7 +637,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -666,10 +664,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -916,9 +914,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1196,7 +1194,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1223,10 +1221,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1475,11 +1473,11 @@
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5078" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.9297" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.1719" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.85156" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.9766" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="8.85156" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.85156" style="1" customWidth="1"/>
   </cols>
@@ -1523,45 +1521,43 @@
       <c r="E2" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="2">
-        <v>12</v>
-      </c>
+      <c r="F2" s="2"/>
       <c r="G2" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="2">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s" s="2">
         <v>14</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="C3" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s" s="2">
         <v>15</v>
       </c>
-      <c r="C3" t="s" s="2">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s" s="2">
-        <v>17</v>
-      </c>
       <c r="G3" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s" s="2">
         <v>10</v>
@@ -1570,21 +1566,21 @@
         <v>11</v>
       </c>
       <c r="F4" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s" s="2">
         <v>10</v>
@@ -1593,21 +1589,21 @@
         <v>11</v>
       </c>
       <c r="F5" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" t="s" s="2">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s" s="2">
         <v>10</v>
@@ -1616,21 +1612,21 @@
         <v>11</v>
       </c>
       <c r="F6" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" t="s" s="2">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s" s="2">
         <v>10</v>
@@ -1639,21 +1635,21 @@
         <v>11</v>
       </c>
       <c r="F7" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s" s="2">
         <v>10</v>
@@ -1662,21 +1658,21 @@
         <v>11</v>
       </c>
       <c r="F8" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s" s="2">
         <v>10</v>
@@ -1685,21 +1681,21 @@
         <v>11</v>
       </c>
       <c r="F9" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" t="s" s="2">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s" s="2">
         <v>10</v>
@@ -1708,21 +1704,21 @@
         <v>11</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" t="s" s="2">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s" s="2">
         <v>10</v>
@@ -1731,21 +1727,21 @@
         <v>11</v>
       </c>
       <c r="F11" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" t="s" s="2">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s" s="2">
         <v>10</v>
@@ -1754,21 +1750,21 @@
         <v>11</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G12" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" ht="13.55" customHeight="1">
       <c r="A13" t="s" s="2">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s" s="2">
         <v>10</v>
@@ -1777,21 +1773,21 @@
         <v>11</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G13" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" ht="13.55" customHeight="1">
       <c r="A14" t="s" s="2">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D14" t="s" s="2">
         <v>10</v>
@@ -1800,21 +1796,21 @@
         <v>11</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G14" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" ht="13.55" customHeight="1">
       <c r="A15" t="s" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s" s="2">
         <v>10</v>
@@ -1823,21 +1819,21 @@
         <v>11</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" ht="13.55" customHeight="1">
       <c r="A16" t="s" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D16" t="s" s="2">
         <v>10</v>
@@ -1846,21 +1842,21 @@
         <v>11</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" ht="13.55" customHeight="1">
       <c r="A17" t="s" s="2">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s" s="2">
         <v>10</v>
@@ -1869,21 +1865,21 @@
         <v>11</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" ht="13.55" customHeight="1">
       <c r="A18" t="s" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D18" t="s" s="2">
         <v>10</v>
@@ -1892,21 +1888,21 @@
         <v>11</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" ht="13.55" customHeight="1">
       <c r="A19" t="s" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D19" t="s" s="2">
         <v>10</v>
@@ -1915,21 +1911,21 @@
         <v>11</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" ht="13.55" customHeight="1">
       <c r="A20" t="s" s="2">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s" s="2">
         <v>10</v>
@@ -1938,21 +1934,21 @@
         <v>11</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" ht="13.55" customHeight="1">
       <c r="A21" t="s" s="2">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D21" t="s" s="2">
         <v>10</v>
@@ -1961,21 +1957,21 @@
         <v>11</v>
       </c>
       <c r="F21" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G21" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" ht="13.55" customHeight="1">
       <c r="A22" t="s" s="2">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D22" t="s" s="2">
         <v>10</v>
@@ -1984,21 +1980,21 @@
         <v>11</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" ht="13.55" customHeight="1">
       <c r="A23" t="s" s="2">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D23" t="s" s="2">
         <v>10</v>
@@ -2007,21 +2003,21 @@
         <v>11</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" ht="13.55" customHeight="1">
       <c r="A24" t="s" s="2">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D24" t="s" s="2">
         <v>10</v>
@@ -2030,21 +2026,21 @@
         <v>11</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" ht="13.55" customHeight="1">
       <c r="A25" t="s" s="2">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D25" t="s" s="2">
         <v>10</v>
@@ -2053,21 +2049,21 @@
         <v>11</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" ht="13.55" customHeight="1">
       <c r="A26" t="s" s="2">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D26" t="s" s="2">
         <v>10</v>
@@ -2076,21 +2072,21 @@
         <v>11</v>
       </c>
       <c r="F26" t="s" s="2">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" ht="13.55" customHeight="1">
       <c r="A27" t="s" s="2">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D27" t="s" s="2">
         <v>10</v>
@@ -2098,45 +2094,43 @@
       <c r="E27" t="s" s="2">
         <v>11</v>
       </c>
-      <c r="F27" t="s" s="2">
-        <v>12</v>
-      </c>
+      <c r="F27" s="2"/>
       <c r="G27" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" ht="13.55" customHeight="1">
       <c r="A28" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s" s="2">
         <v>66</v>
       </c>
-      <c r="B28" t="s" s="2">
+      <c r="G28" t="s" s="2">
         <v>67</v>
-      </c>
-      <c r="C28" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="D28" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="E28" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="F28" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="G28" t="s" s="2">
-        <v>70</v>
       </c>
     </row>
     <row r="29" ht="13.55" customHeight="1">
       <c r="A29" t="s" s="2">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s" s="2">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="D29" t="s" s="2">
         <v>10</v>
@@ -2145,21 +2139,21 @@
         <v>11</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" t="s" s="2">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="D30" t="s" s="2">
         <v>10</v>
@@ -2168,21 +2162,21 @@
         <v>11</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" ht="13.55" customHeight="1">
       <c r="A31" t="s" s="2">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="D31" t="s" s="2">
         <v>10</v>
@@ -2191,148 +2185,144 @@
         <v>11</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" ht="13.55" customHeight="1">
       <c r="A32" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>76</v>
+      </c>
+      <c r="D32" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="E32" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="B32" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="C32" t="s" s="2">
-        <v>79</v>
-      </c>
-      <c r="D32" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="E32" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="F32" t="s" s="2">
-        <v>12</v>
-      </c>
+      <c r="F32" s="2"/>
       <c r="G32" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" ht="13.55" customHeight="1">
       <c r="A33" t="s" s="2">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D33" t="s" s="2">
         <v>10</v>
       </c>
       <c r="E33" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="F33" t="s" s="2">
-        <v>12</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F33" s="2"/>
       <c r="G33" t="s" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" ht="13.55" customHeight="1">
       <c r="A34" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="B34" t="s" s="2">
+      <c r="E34" t="s" s="2">
+        <v>77</v>
+      </c>
+      <c r="F34" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="C34" t="s" s="2">
+      <c r="G34" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="D34" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="E34" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="F34" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="G34" t="s" s="2">
-        <v>89</v>
       </c>
     </row>
     <row r="35" ht="13.55" customHeight="1">
       <c r="A35" t="s" s="2">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="D35" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="E35" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="G35" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="D35" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="E35" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="F35" t="s" s="2">
-        <v>88</v>
-      </c>
-      <c r="G35" t="s" s="2">
-        <v>89</v>
       </c>
     </row>
     <row r="36" ht="13.55" customHeight="1">
       <c r="A36" t="s" s="2">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C36" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="D36" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="E36" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="G36" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="D36" t="s" s="2">
-        <v>10</v>
-      </c>
-      <c r="E36" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="F36" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="G36" t="s" s="2">
-        <v>89</v>
       </c>
     </row>
     <row r="37" ht="17" customHeight="1">
       <c r="A37" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>93</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="D37" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="E37" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s" s="3">
         <v>95</v>
       </c>
-      <c r="B37" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="C37" t="s" s="2">
+      <c r="G37" t="s" s="2">
         <v>86</v>
-      </c>
-      <c r="D37" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="E37" t="s" s="2">
-        <v>11</v>
-      </c>
-      <c r="F37" t="s" s="3">
-        <v>98</v>
-      </c>
-      <c r="G37" t="s" s="2">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>